<commit_message>
adding more source files to project. Parser, data files and main testing file
</commit_message>
<xml_diff>
--- a/Project/data/WGUPS Package File.xlsx
+++ b/Project/data/WGUPS Package File.xlsx
@@ -5,15 +5,15 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lo850n/Downloads/WGU_C950/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lo850n/Desktop/Leo/CC950/WGU_C950/Project/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76E834BC-90E5-C242-B29C-029E93FC4CFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA4EE7A7-B0DB-3545-BB7C-FB6A5791E036}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3420" yWindow="840" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="packages" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -541,7 +541,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H41"/>
   <sheetViews>
-    <sheetView tabSelected="1" showWhiteSpace="0" view="pageLayout" zoomScale="135" zoomScaleNormal="100" zoomScalePageLayoutView="135" workbookViewId="0">
+    <sheetView tabSelected="1" showWhiteSpace="0" view="pageLayout" topLeftCell="A5" zoomScale="135" zoomScaleNormal="100" zoomScalePageLayoutView="135" workbookViewId="0">
       <selection activeCell="H43" sqref="H43"/>
     </sheetView>
   </sheetViews>
@@ -1572,6 +1572,52 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Vendor xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41">N/A</Vendor>
+    <Course_x0020_title xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41" xsi:nil="true"/>
+    <Launch_x0020_Date xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41" xsi:nil="true"/>
+    <Discipline xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41" xsi:nil="true"/>
+    <Course_x0020_short_x0020_name xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41" xsi:nil="true"/>
+    <SME xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41" xsi:nil="true"/>
+    <Course_x0020_code xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41" xsi:nil="true"/>
+    <qrac xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41" xsi:nil="true"/>
+    <Step_x0020_Completed xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41">
+      <Value>N/A</Value>
+    </Step_x0020_Completed>
+    <Course_x0020_number xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41" xsi:nil="true"/>
+    <d5fh xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41" xsi:nil="true"/>
+    <Publication_x0020_Date xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41" xsi:nil="true"/>
+    <Assessment_x0020_Type xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41">
+      <Value>Objective</Value>
+    </Assessment_x0020_Type>
+    <Editor0 xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Editor0>
+    <Doc_x0020_Type xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41"/>
+    <Performance_x0020_Steps_x0020_Completed xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41">
+      <Value>N/A</Value>
+    </Performance_x0020_Steps_x0020_Completed>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C39F2A75005F2D43B30369DAED2CCB1C" ma:contentTypeVersion="40" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="67abd11da167d8eab610c259a823e4c7">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="0feec74c-ecc7-44c3-9c64-3623cf89ed41" xmlns:ns3="1f707338-ea0f-4fe5-baee-59b996692b22" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1d3ab84303ed41503c975572ff37e680" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -2009,53 +2055,33 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8ACC0CE6-074E-44A2-B54E-38496285A228}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="cf660112-59e0-48e5-9b60-3f2262d4e05d"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="0feec74c-ecc7-44c3-9c64-3623cf89ed41"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Vendor xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41">N/A</Vendor>
-    <Course_x0020_title xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41" xsi:nil="true"/>
-    <Launch_x0020_Date xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41" xsi:nil="true"/>
-    <Discipline xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41" xsi:nil="true"/>
-    <Course_x0020_short_x0020_name xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41" xsi:nil="true"/>
-    <SME xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41" xsi:nil="true"/>
-    <Course_x0020_code xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41" xsi:nil="true"/>
-    <qrac xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41" xsi:nil="true"/>
-    <Step_x0020_Completed xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41">
-      <Value>N/A</Value>
-    </Step_x0020_Completed>
-    <Course_x0020_number xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41" xsi:nil="true"/>
-    <d5fh xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41" xsi:nil="true"/>
-    <Publication_x0020_Date xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41" xsi:nil="true"/>
-    <Assessment_x0020_Type xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41">
-      <Value>Objective</Value>
-    </Assessment_x0020_Type>
-    <Editor0 xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Editor0>
-    <Doc_x0020_Type xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41"/>
-    <Performance_x0020_Steps_x0020_Completed xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41">
-      <Value>N/A</Value>
-    </Performance_x0020_Steps_x0020_Completed>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D0E77ABB-EDCD-4FE8-A23F-B30F5B1F6DEF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5E8A0206-F67A-481E-AE05-AF5EAD7E6628}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2073,30 +2099,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D0E77ABB-EDCD-4FE8-A23F-B30F5B1F6DEF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8ACC0CE6-074E-44A2-B54E-38496285A228}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="cf660112-59e0-48e5-9b60-3f2262d4e05d"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="0feec74c-ecc7-44c3-9c64-3623cf89ed41"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>